<commit_message>
Reportes normalizacion y modelo
</commit_message>
<xml_diff>
--- a/Normalizaciòn y diseño base de datos proyecto 3.xlsx
+++ b/Normalizaciòn y diseño base de datos proyecto 3.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37f9fb9f87cc4ef1/Universidad/Tercer año/Primer Semestre/Base de datos 1/Proyectos/Proyecto3-GIT/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_946C61843A097EBECDE0A154CC20482569B25F17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977AF0E6-5E11-4300-9EB1-6F0DD759B9AF}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Entidades</t>
   </si>
@@ -167,37 +176,53 @@
   </si>
   <si>
     <t>accion</t>
+  </si>
+  <si>
+    <t>busquedas</t>
+  </si>
+  <si>
+    <t>busqueda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -217,43 +242,58 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -443,427 +483,482 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.13"/>
-    <col customWidth="1" min="2" max="2" width="15.75"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="s">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="s">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="4" t="s">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="4" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="2" t="s">
+      <c r="B52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="2" t="s">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="2" t="s">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="s">
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="4" t="s">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2" t="s">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A58:C58"/>
+  <mergeCells count="21">
+    <mergeCell ref="A70:C70"/>
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A67:C67"/>
     <mergeCell ref="A64:E64"/>
@@ -874,7 +969,18 @@
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>